<commit_message>
neo4j backend overhaul finished
Much faster now. Also improved parser speed for frontend setup.
Setup should work now as well.
</commit_message>
<xml_diff>
--- a/data/ingest/hss-txtwtns.xlsx
+++ b/data/ingest/hss-txtwtns.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kraus0001\PycharmProjects\pamphilus_db\data\ingest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kraus0001/Coding/pamphilus_db/data/ingest/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F34C8E-B035-AE49-9610-CF3E73A80DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22800" yWindow="9105" windowWidth="6000" windowHeight="9780"/>
+    <workbookView xWindow="10480" yWindow="500" windowWidth="30240" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -860,7 +855,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -978,26 +973,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:N62" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:N62"/>
-  <sortState ref="A2:L62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:N62" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:N62" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L62">
     <sortCondition ref="A1:A62"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Abbreviation" dataDxfId="12"/>
-    <tableColumn id="2" name="Signature" dataDxfId="11"/>
-    <tableColumn id="3" name="Name" dataDxfId="10"/>
-    <tableColumn id="4" name="TxtWitID" dataDxfId="9"/>
-    <tableColumn id="5" name="TextFamily" dataDxfId="8"/>
-    <tableColumn id="6" name="TxtFamID" dataDxfId="7"/>
-    <tableColumn id="7" name="Matter" dataDxfId="6"/>
-    <tableColumn id="8" name="Current Location" dataDxfId="5"/>
-    <tableColumn id="9" name="Link" dataDxfId="4"/>
-    <tableColumn id="10" name="AuthURI" dataDxfId="3"/>
-    <tableColumn id="11" name="Spalte1" dataDxfId="2"/>
-    <tableColumn id="12" name="handritURL"/>
-    <tableColumn id="13" name="lang" dataDxfId="1"/>
-    <tableColumn id="14" name="Meter" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Abbreviation" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Signature" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TxtWitID" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TextFamily" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TxtFamID" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Matter" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Current Location" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Link" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="AuthURI" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Spalte1" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="handritURL"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="lang" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Meter" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1299,29 +1294,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -1365,7 +1360,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>245</v>
       </c>
@@ -1398,7 +1393,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>251</v>
       </c>
@@ -1431,7 +1426,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
@@ -1464,7 +1459,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
@@ -1497,7 +1492,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -1530,7 +1525,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -1563,7 +1558,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
@@ -1596,7 +1591,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -1629,7 +1624,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1662,7 +1657,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1695,7 +1690,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1728,7 +1723,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -1761,7 +1756,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -1794,7 +1789,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1827,7 +1822,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
@@ -1860,7 +1855,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
@@ -1893,7 +1888,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>91</v>
       </c>
@@ -1926,7 +1921,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>91</v>
       </c>
@@ -1959,7 +1954,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>91</v>
       </c>
@@ -1992,7 +1987,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>91</v>
       </c>
@@ -2027,7 +2022,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>91</v>
       </c>
@@ -2060,7 +2055,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>91</v>
       </c>
@@ -2091,7 +2086,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -2126,7 +2121,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -2161,7 +2156,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -2196,7 +2191,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2231,7 +2226,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
@@ -2264,7 +2259,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -2299,7 +2294,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -2334,7 +2329,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -2369,7 +2364,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -2402,7 +2397,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -2435,7 +2430,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -2471,7 +2466,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -2508,7 +2503,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -2541,7 +2536,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
@@ -2574,7 +2569,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>70</v>
       </c>
@@ -2607,7 +2602,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
@@ -2642,7 +2637,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>70</v>
       </c>
@@ -2677,7 +2672,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -2713,7 +2708,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -2750,7 +2745,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -2787,7 +2782,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -2822,7 +2817,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -2855,7 +2850,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -2890,7 +2885,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -2923,7 +2918,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -2956,7 +2951,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -2989,7 +2984,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -3024,7 +3019,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -3061,7 +3056,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>25</v>
       </c>
@@ -3098,7 +3093,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>25</v>
       </c>
@@ -3131,7 +3126,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
@@ -3164,7 +3159,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -3199,7 +3194,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>25</v>
       </c>
@@ -3234,7 +3229,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>25</v>
       </c>
@@ -3267,7 +3262,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>25</v>
       </c>
@@ -3300,7 +3295,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>25</v>
       </c>
@@ -3333,7 +3328,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>25</v>
       </c>
@@ -3368,7 +3363,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>25</v>
       </c>
@@ -3402,7 +3397,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
@@ -3438,16 +3433,16 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J26" r:id="rId1" tooltip="http://d-nb.info/gnd/118704710"/>
-    <hyperlink ref="J29" r:id="rId2" tooltip="http://d-nb.info/gnd/100963927"/>
-    <hyperlink ref="J31" r:id="rId3"/>
-    <hyperlink ref="J52" r:id="rId4"/>
-    <hyperlink ref="J51" r:id="rId5" tooltip="http://d-nb.info/gnd/118704710"/>
-    <hyperlink ref="J56" r:id="rId6" tooltip="http://d-nb.info/gnd/118704710"/>
-    <hyperlink ref="J55" r:id="rId7" tooltip="http://d-nb.info/gnd/100963927"/>
-    <hyperlink ref="J39" r:id="rId8" tooltip="http://d-nb.info/gnd/118590995"/>
-    <hyperlink ref="J40" r:id="rId9" tooltip="http://d-nb.info/gnd/118590995"/>
-    <hyperlink ref="J35" r:id="rId10"/>
+    <hyperlink ref="J26" r:id="rId1" tooltip="http://d-nb.info/gnd/118704710" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J29" r:id="rId2" tooltip="http://d-nb.info/gnd/100963927" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J31" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J52" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J51" r:id="rId5" tooltip="http://d-nb.info/gnd/118704710" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J56" r:id="rId6" tooltip="http://d-nb.info/gnd/118704710" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J55" r:id="rId7" tooltip="http://d-nb.info/gnd/100963927" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="J39" r:id="rId8" tooltip="http://d-nb.info/gnd/118590995" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J40" r:id="rId9" tooltip="http://d-nb.info/gnd/118590995" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J35" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId11"/>

</xml_diff>